<commit_message>
Make code more independent of requested energy types
Until now, heat, hot water and electricity profiles had to be
created and included in the output. Now lpagg should work even if
only e.g. electricity profiles are requested.

Total annual energy values missing from the houses input data
(or set to NaN) result in those profiles not being created.

This causes a breaking change:
For households, VDI 4655 provides default values for annual hot
water and electricity demands. If missing from the input data,
those were automatically calculated. Now those defaults are only
calculated if their annual value is a string, e.g. 'calculate'

See this example for the configuration.yaml

houses:
    EFH:
        Q_Heiz_a: 6000  # Value given, profile is created
        Q_TWW_a: calculate  # VDI4655 default is calculated
        # W_a:  # electricity profile is not created
</commit_message>
<xml_diff>
--- a/lpagg/examples/VDI_4655_houses_example.xlsx
+++ b/lpagg/examples/VDI_4655_houses_example.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDEB822-7517-4CED-8598-060FB840A7FE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB248E4-630D-42E5-A773-97E484B1A22B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26385" yWindow="8145" windowWidth="25470" windowHeight="18495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>EFH</t>
   </si>
@@ -28,9 +28,6 @@
     <t>MFH</t>
   </si>
   <si>
-    <t>Buero</t>
-  </si>
-  <si>
     <t>Handel</t>
   </si>
   <si>
@@ -61,13 +58,19 @@
     <t>sigma</t>
   </si>
   <si>
-    <t>G1G</t>
-  </si>
-  <si>
-    <t>G4G</t>
-  </si>
-  <si>
     <t>Q_Kalt_a</t>
+  </si>
+  <si>
+    <t>calculate</t>
+  </si>
+  <si>
+    <t>GHD/G1</t>
+  </si>
+  <si>
+    <t>GHA/G4</t>
+  </si>
+  <si>
+    <t>Büro</t>
   </si>
 </sst>
 </file>
@@ -388,15 +391,15 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -404,15 +407,15 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>4</v>
       </c>
       <c r="B2">
         <v>6000</v>
@@ -427,9 +430,9 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <v>7000</v>
@@ -438,9 +441,15 @@
         <v>43000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
       </c>
       <c r="D4">
         <v>1500</v>
@@ -449,9 +458,15 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
       </c>
       <c r="D5">
         <v>60000</v>
@@ -460,9 +475,9 @@
         <v>110000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -477,9 +492,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
@@ -488,15 +503,15 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -511,9 +526,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -528,26 +543,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>11</v>
-      </c>
-      <c r="B10">
-        <v>24</v>
-      </c>
-      <c r="C10">
-        <v>24</v>
-      </c>
-      <c r="D10">
-        <v>4</v>
-      </c>
-      <c r="E10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>12</v>
       </c>
       <c r="B11">
         <v>4</v>
@@ -564,5 +579,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>